<commit_message>
feat: Add waliKelas details to the kelas API response, improve frontend API response typing, and update kelas data.
</commit_message>
<xml_diff>
--- a/data-import/data_kelas.xlsx
+++ b/data-import/data_kelas.xlsx
@@ -32,12 +32,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -446,10 +442,10 @@
         <v>Akuntansi</v>
       </c>
       <c r="F2" t="str">
-        <v/>
+        <v>0000000000000066</v>
       </c>
       <c r="G2" t="str">
-        <v/>
+        <v>M. Fais Jainuddin, S.Pd</v>
       </c>
     </row>
     <row r="3">
@@ -469,10 +465,10 @@
         <v>Teknik Kendaraan Ringan</v>
       </c>
       <c r="F3" t="str">
-        <v/>
+        <v>5736762663300210</v>
       </c>
       <c r="G3" t="str">
-        <v/>
+        <v>Nunung Indrawati, S.Pd.</v>
       </c>
     </row>
     <row r="4">
@@ -492,10 +488,10 @@
         <v>Teknik Komputer dan Jaringan</v>
       </c>
       <c r="F4" t="str">
-        <v/>
+        <v>0000000000000044</v>
       </c>
       <c r="G4" t="str">
-        <v/>
+        <v>Zulfi Amaliyah, S.Kom.</v>
       </c>
     </row>
     <row r="5">
@@ -515,10 +511,10 @@
         <v>Akuntansi</v>
       </c>
       <c r="F5" t="str">
-        <v/>
+        <v>0000000000000006</v>
       </c>
       <c r="G5" t="str">
-        <v/>
+        <v>Mulyono, S.Th.</v>
       </c>
     </row>
     <row r="6">
@@ -538,10 +534,10 @@
         <v>Teknik Kendaraan Ringan</v>
       </c>
       <c r="F6" t="str">
-        <v/>
+        <v>5040758659300040</v>
       </c>
       <c r="G6" t="str">
-        <v/>
+        <v>Nurmala Evayanti S.Pd.</v>
       </c>
     </row>
     <row r="7">
@@ -561,10 +557,10 @@
         <v>Teknik Komputer dan Jaringan</v>
       </c>
       <c r="F7" t="str">
-        <v/>
+        <v>00000000000000022222</v>
       </c>
       <c r="G7" t="str">
-        <v/>
+        <v>Fera Mega Haristina, S.Tr.Kom.</v>
       </c>
     </row>
     <row r="8">
@@ -584,10 +580,10 @@
         <v>Akuntansi</v>
       </c>
       <c r="F8" t="str">
-        <v/>
+        <v>00000000000000004</v>
       </c>
       <c r="G8" t="str">
-        <v/>
+        <v>Imtiana, S.Pd.</v>
       </c>
     </row>
     <row r="9">
@@ -607,10 +603,10 @@
         <v>Teknik Kendaraan Ringan</v>
       </c>
       <c r="F9" t="str">
-        <v/>
+        <v>0000000023232323</v>
       </c>
       <c r="G9" t="str">
-        <v/>
+        <v>Frances Laurence Setyo Budi, S.Pd.</v>
       </c>
     </row>
     <row r="10">
@@ -630,10 +626,10 @@
         <v>Teknik Komputer dan Jaringan</v>
       </c>
       <c r="F10" t="str">
-        <v/>
+        <v>0000000000000010044</v>
       </c>
       <c r="G10" t="str">
-        <v/>
+        <v>Udayani, S.Pd.</v>
       </c>
     </row>
   </sheetData>

</xml_diff>